<commit_message>
Modify the code for better view
</commit_message>
<xml_diff>
--- a/amenities.xlsx
+++ b/amenities.xlsx
@@ -31,13 +31,22 @@
     <t>Dryer</t>
   </si>
   <si>
+    <t>Cat(s)</t>
+  </si>
+  <si>
     <t>Dog(s)</t>
   </si>
   <si>
     <t>Washer</t>
   </si>
   <si>
-    <t>Cat(s)</t>
+    <t>Kitchen</t>
+  </si>
+  <si>
+    <t>Shampoo</t>
+  </si>
+  <si>
+    <t>Hangers</t>
   </si>
   <si>
     <t>Heating</t>
@@ -49,15 +58,6 @@
     <t>Doorman</t>
   </si>
   <si>
-    <t>Hangers</t>
-  </si>
-  <si>
-    <t>Shampoo</t>
-  </si>
-  <si>
-    <t>Kitchen</t>
-  </si>
-  <si>
     <t>Internet</t>
   </si>
   <si>
@@ -67,12 +67,12 @@
     <t>Breakfast</t>
   </si>
   <si>
+    <t>Essentials</t>
+  </si>
+  <si>
     <t>Hair Dryer</t>
   </si>
   <si>
-    <t>Essentials</t>
-  </si>
-  <si>
     <t>Safety Card</t>
   </si>
   <si>
@@ -109,16 +109,16 @@
     <t>Wireless Internet</t>
   </si>
   <si>
+    <t>Suitable for Events</t>
+  </si>
+  <si>
     <t>Family/Kid Friendly</t>
   </si>
   <si>
-    <t>Suitable for Events</t>
+    <t>Lock on Bedroom Door</t>
   </si>
   <si>
     <t>Elevator in Building</t>
-  </si>
-  <si>
-    <t>Lock on Bedroom Door</t>
   </si>
   <si>
     <t>Wheelchair Accessible</t>

</xml_diff>